<commit_message>
LMT-D misalignment<< same channels for LMT-A
</commit_message>
<xml_diff>
--- a/freeSpaceLoss.xlsx
+++ b/freeSpaceLoss.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bxin/wavefront/gmtScratchBook/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89831021-4B93-B146-8DBE-6EAB79A10318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF1FD41-38B0-5F4F-8F4A-4DC0300F7E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11680" yWindow="-20040" windowWidth="26040" windowHeight="13600" xr2:uid="{88F2F4A2-56F8-BA4A-B393-B0681C843647}"/>
+    <workbookView xWindow="24260" yWindow="-23580" windowWidth="32080" windowHeight="15960" xr2:uid="{88F2F4A2-56F8-BA4A-B393-B0681C843647}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,9 +62,6 @@
     <t>NA*f</t>
   </si>
   <si>
-    <t>CA req</t>
-  </si>
-  <si>
     <t>Beam radius (zmx)</t>
   </si>
   <si>
@@ -137,9 +134,6 @@
     <t>CAD (retaining ring)</t>
   </si>
   <si>
-    <t>CA (Thorlabs 90% visible portion of lens)</t>
-  </si>
-  <si>
     <t>Beam radius (zmx) (1m)</t>
   </si>
   <si>
@@ -161,7 +155,13 @@
     <t>focal length</t>
   </si>
   <si>
-    <t>CA (zmx model from Thorlabs)</t>
+    <t>CA Radius (Thorlabs 90% visible portion of lens)</t>
+  </si>
+  <si>
+    <t>CA Radius req</t>
+  </si>
+  <si>
+    <t>CA Radius (zmx model from Thorlabs)</t>
   </si>
 </sst>
 </file>
@@ -169,9 +169,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -195,12 +195,6 @@
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -423,9 +417,57 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -438,61 +480,13 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -519,9 +513,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -559,7 +553,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -665,7 +659,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -807,7 +801,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -832,7 +826,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J2" sqref="J2:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,95 +834,95 @@
     <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="133" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="155" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>35</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="R1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="19" t="s">
-        <v>18</v>
-      </c>
       <c r="T1" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>23</v>
-      </c>
-      <c r="W1" s="19" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:24" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="34">
         <v>1.8</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="44">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="37">
         <f>D4*E4</f>
         <v>2.8125</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="33">
+      <c r="H2" s="31">
         <v>3</v>
       </c>
       <c r="I2" s="3"/>
-      <c r="J2" s="33">
+      <c r="J2" s="31">
         <v>3.25</v>
       </c>
       <c r="K2" s="4">
@@ -947,18 +941,18 @@
         <v>2.95</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="27" t="s">
         <v>7</v>
-      </c>
-      <c r="Q2" s="30" t="s">
-        <v>8</v>
       </c>
       <c r="R2">
         <v>1.5</v>
       </c>
       <c r="S2" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="23">
+        <v>18</v>
+      </c>
+      <c r="T2" s="30">
         <v>0.6</v>
       </c>
       <c r="U2">
@@ -972,22 +966,22 @@
         <v>0.35</v>
       </c>
       <c r="X2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="67" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="34"/>
+      <c r="A3" s="32"/>
       <c r="B3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="45"/>
+        <v>8</v>
+      </c>
+      <c r="C3" s="35"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="15"/>
-      <c r="H3" s="34"/>
+      <c r="H3" s="32"/>
       <c r="I3" s="15"/>
-      <c r="J3" s="34"/>
+      <c r="J3" s="32"/>
       <c r="K3" s="7">
         <v>2.6259999999999999</v>
       </c>
@@ -1001,11 +995,11 @@
         <v>1.282</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="P3" s="9"/>
-      <c r="Q3" s="31"/>
-      <c r="T3" s="23"/>
+      <c r="Q3" s="28"/>
+      <c r="T3" s="30"/>
       <c r="U3">
         <f>(M3-K3)/K3*C2</f>
         <v>-7.9512566641279592E-2</v>
@@ -1019,31 +1013,31 @@
       </c>
     </row>
     <row r="4" spans="1:24" ht="67" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
+      <c r="A4" s="33"/>
       <c r="B4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="29"/>
-      <c r="D4" s="39">
+        <v>10</v>
+      </c>
+      <c r="C4" s="36"/>
+      <c r="D4" s="25">
         <v>0.15</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="25">
         <v>18.75</v>
       </c>
-      <c r="F4" s="46"/>
+      <c r="F4" s="39"/>
       <c r="G4" s="16">
         <v>2.6</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="33"/>
       <c r="I4" s="16">
         <v>2.9</v>
       </c>
-      <c r="J4" s="35"/>
+      <c r="J4" s="33"/>
       <c r="K4" s="10">
         <v>2.62</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M4" s="10">
         <v>5.0350000000000001</v>
@@ -1055,34 +1049,34 @@
         <v>173.529</v>
       </c>
       <c r="P4" s="9"/>
-      <c r="Q4" s="32"/>
-      <c r="T4" s="23"/>
+      <c r="Q4" s="29"/>
+      <c r="T4" s="30"/>
       <c r="W4">
         <v>0.2</v>
       </c>
     </row>
     <row r="5" spans="1:24" ht="23" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
-        <v>13</v>
+      <c r="A5" s="40" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="27">
+        <v>5</v>
+      </c>
+      <c r="C5" s="43">
         <v>3.5</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="41">
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="44">
         <f>D7*E7</f>
         <v>8.9112000000000009</v>
       </c>
       <c r="G5" s="20"/>
-      <c r="H5" s="24">
+      <c r="H5" s="40">
         <v>7</v>
       </c>
       <c r="I5" s="11"/>
-      <c r="J5" s="24">
+      <c r="J5" s="40">
         <v>10</v>
       </c>
       <c r="K5" s="12">
@@ -1101,18 +1095,18 @@
         <v>13.359</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="R5" s="17">
         <v>3.5</v>
       </c>
       <c r="S5" t="s">
-        <v>20</v>
-      </c>
-      <c r="T5" s="23">
+        <v>19</v>
+      </c>
+      <c r="T5" s="30">
         <v>6.4</v>
       </c>
       <c r="U5">
@@ -1124,18 +1118,18 @@
       </c>
     </row>
     <row r="6" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="42"/>
+        <v>8</v>
+      </c>
+      <c r="C6" s="35"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="45"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="25"/>
+      <c r="H6" s="41"/>
       <c r="I6" s="17"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="41"/>
       <c r="K6" s="12">
         <v>5.1840000000000002</v>
       </c>
@@ -1153,29 +1147,29 @@
       </c>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
-      <c r="T6" s="23"/>
+      <c r="T6" s="30"/>
     </row>
     <row r="7" spans="1:24" ht="67" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26"/>
+      <c r="A7" s="42"/>
       <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="39">
+        <v>10</v>
+      </c>
+      <c r="C7" s="36"/>
+      <c r="D7" s="25">
         <v>0.24</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="25">
         <v>37.130000000000003</v>
       </c>
-      <c r="F7" s="43"/>
+      <c r="F7" s="46"/>
       <c r="G7" s="22">
         <v>8.1</v>
       </c>
-      <c r="H7" s="26"/>
+      <c r="H7" s="42"/>
       <c r="I7" s="18">
         <v>9</v>
       </c>
-      <c r="J7" s="26"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="12">
         <v>5.17</v>
       </c>
@@ -1183,7 +1177,7 @@
         <v>0.74199999999999999</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N7" s="7">
         <v>130.94399999999999</v>
@@ -1193,10 +1187,16 @@
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
-      <c r="T7" s="23"/>
+      <c r="T7" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="T5:T7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="J5:J7"/>
     <mergeCell ref="Q2:Q4"/>
     <mergeCell ref="T2:T4"/>
     <mergeCell ref="A2:A4"/>
@@ -1204,12 +1204,6 @@
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="H2:H4"/>
     <mergeCell ref="J2:J4"/>
-    <mergeCell ref="T5:T7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="J5:J7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>